<commit_message>
Adding my powerpoint and some graphs
</commit_message>
<xml_diff>
--- a/Output/Variety vs Price.xlsx
+++ b/Output/Variety vs Price.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin.Ford\Documents\Bootcamp Project 1\PourTaste\Output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EB3B4C-396B-4145-9B27-79455CC642CA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -133,8 +139,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,15 +157,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF404040"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -168,9 +180,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -182,22 +192,207 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="12">
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF404040"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{A22854F7-4348-4FC8-86E6-E554B3CFD9C4}">
+      <tableStyleElement type="wholeTable" dxfId="11"/>
+      <tableStyleElement type="headerRow" dxfId="10"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71CB930D-BE48-417F-AD2A-99CBE247154C}" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="9">
+  <autoFilter ref="A1:F11" xr:uid="{1AEAA846-45E4-4465-9941-13152CE59C7B}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{E3C63F88-025F-42D3-8667-DDBC0F74C14B}" name="variety" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{DF98291E-650D-4D74-85C2-A7C84B424354}" name="Number of Wines in Dataframe" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{CF96742D-30D9-4445-82A2-0A70C160F4C9}" name="Average Price" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{4C9C3C0F-CE3F-4ABE-BE83-27E84DFFCE53}" name="Cheapest Bottle" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{9CC3508F-49D3-4E26-93AD-0A68CE26145A}" name="Most Expensive Bottle" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{578628EA-7CD8-4E39-AFE9-08D49AC8413A}" name="Average Point Value" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -243,7 +438,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,9 +470,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -309,6 +522,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -484,234 +715,250 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.46484375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.73046875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>12787</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>11080</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="4">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>9386</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>8476</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>5340</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="4">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>4972</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="4">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>4783</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="4">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>4086</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="4">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>3262</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="4">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4">
         <v>3062</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="4">
         <v>87</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C2:F11" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>